<commit_message>
Switch to llm agents
</commit_message>
<xml_diff>
--- a/results/lecture_1_reviews.xlsx
+++ b/results/lecture_1_reviews.xlsx
@@ -521,33 +521,31 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C2" t="n">
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Good technical implementation with minor areas for improvement. Excellent code style and naming conventions. Excellent documentation with comprehensive docstrings. Performance appears adequate for the task requirements.</t>
+          <t>\n     - Catch ValueError for invalid float conversion.\n     - Catch the specific exception you raise on divide-by-zero (ValueError or better use ZeroDivisionError).\n   - Consider letting unexpected exceptions propagate (or at least re-raise after logging) during development.\n\n2. Consistency for divide-by-zero\n   - Python’s built-in division raises ZeroDivisionError. Consider raising ZeroDivisionError in divide(a, b) instead of ValueError to be consistent with standard practice:\n     raise ZeroDivisionError("Cannot divide by zero")\n\n3. Input handling / UX\n   - Trim user input for the operation: operation = input(...).strip()\n   - Consider accepting alternative symbols (e.g., \'x\' or \'X\' for multiplication) or validating more explicitly and informing the user.\n   - You may want to loop so the user can perform multiple calculations in one run, and provide a way to quit.\n\n4. Minor robustness notes\n   - Checking b == 0 is fine for direct zeros. If you intend to handle floats that are extremely close to zero, you might consider an epsilon check. For this assignment it’s not necessary, but worth noting.\n   - Consider documenting expected input formats in the module or main docstring.\n\n5. Documentation &amp; style\n   - Add a module-level docstring briefly describing the script.\n   - Consider type hints for function signatures for clarity:\n     def add(a: float, b: float) -&gt; float:\n   - The code is already readable; consider adding a short comment for the main flow or a small README if this were part of a larger project.\n\n6. Tests\n   - Add unit tests (pytest/unittest) for the four operations, including a test for division by zero. This improves correctness assurance and is an excellent habit.\n\nExample small improvements\n- Strip input, catch specific exceptions, and use ZeroDivisionError:\n  operation = input("Enter operation (+, -, *, /): ").strip()\n  try:\n      num1 = float(input("Enter first number: "))\n      num2 = float(input("Enter second number: "))\n  except ValueError:\n      print("Error: Please enter valid numbers.")\n      return\n\n  try:\n      if operation == \'+\':\n          result = add(num1, num2)\n      ...\n      elif operation == \'/\':\n          result = divide(num1, num2)\n  except ZeroDivisionError:\n      print("Error: Cannot divide by zero")\n\nFinal summary\n- Functional and well-documented at the function level.\n- A few small improvements around exception specificity, input trimming, minor style touches, and tests would make this excellent.\n- Final overall score: 91 — very good work.'</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" t="n">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I2" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>45913.76392361111</v>
+        <v>45914.6452199074</v>
       </c>
     </row>
     <row r="3">
@@ -559,33 +557,31 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C3" t="n">
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Good technical implementation with minor areas for improvement. Excellent code style and naming conventions. Excellent documentation with comprehensive docstrings. Performance appears adequate for the task requirements.</t>
+          <t>Student and GradeManager classes behave as expected.\n- add_grade validates grade range (0–100).\n- get_average_grade and get_grade_report handle the empty-grades case gracefully.\n- Docstrings for all public classes and methods are provided.\n- Readable and well organized; variable and method names are descriptive.\n\nSuggested improvements and edge cases\n1. Class-average definition\n   - Current implementation computes class average as the mean of each student’s average:\n     total = average(student_i_average) over students.\n     This treats each student equally even if they have different numbers of grades. That is valid in some contexts but often you\'d want the average of all individual grades across the class (i.e., weight each grade equally). Consider documenting which definition you use or provide both options (per-student average vs. per-grade average).\n   - If you intend to exclude students with no grades from the class average, filter them out; currently a student with no grades contributes 0 to the class average which may skew results.\n\n2. Duplicate student IDs\n   - add_student silently overwrites any existing student with the same student_id. It\'s better to:\n     - raise an error (ValueError) if a duplicate ID is added, or\n     - return the existing student and avoid creating a new one, or\n     - provide an update method and document behavior.\n   - At minimum, consider checking and documenting behavior.\n\n3. Type hints and input validation\n   - Add type hints for function signatures (PEP 484) to improve readability and help static analysis tools.\n   - You might validate that subject is a non-empty string and grade is numeric (float/int) before storing.\n\n4. API niceties\n   - Implement __repr__ or __str__ for Student to make debugging and printing nicer (e.g., Student(name=\'Alice\', id=\'S001\')).\n   - Consider methods to remove or update grades, list subjects, or export/import student data.\n   - Consider adding unit tests for core behavior and edge cases (no grades, duplicate IDs, invalid grades).\n\n5. Separation of concerns\n   - main() includes interactive/demo code which is fine for a script, but if this module is intended as a reusable library, consider moving demo code to a separate script or protecting main (already done using if __name__ == "__main__":). Also consider making printing optional or providing a CLI/formatter.\n\n6. Small style/format suggestions\n   - When computing averages, you could use statistics.mean for readability.\n   - When there are no students or grades, decide whether to return None (to indicate absence) rather than 0, depending on the API contract; returning 0 is okay but document it clearly.\n   - Add unit tests or a README describing intended behavior (how class average is computed, how duplicates are handled, etc.).\n\nExample changes (brief)\n- Exclude students with no grades from class average:\n  students_with_grades = [s for s in self.students.values() if s.grades]\n  if not students_with_grades:\n      return 0\n  total_average = sum(s.get_average_grade() for s in students_with_grades)\n  return total_average / len(students_with_grades)\n\n- Prevent overwriting student IDs:\n  if student_id in self.students:\n      raise ValueError(f"Student with ID {student_id} already exists.")\n  student = Student(name, student_id)\n  self.students[student_id] = student\n\nSummary\n- The submission meets the assignment and is implemented cleanly.\n- Minor improvements would make the code more robust and production-ready: clarify class-average definition, handle duplicate IDs, add type hints and more validation, and possibly add __repr__ and unit tests.\n\nWell done — solid implementation with clear scope.'</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G3" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I3" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>45913.76392361111</v>
+        <v>45914.6452199074</v>
       </c>
     </row>
     <row r="4">
@@ -597,10 +593,8 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C4" t="n">
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>93</v>
@@ -635,10 +629,8 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C5" t="n">
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>74</v>

</xml_diff>

<commit_message>
Add downloading github repos feature and checking lecture and tasks from them
</commit_message>
<xml_diff>
--- a/results/lecture_1_reviews.xlsx
+++ b/results/lecture_1_reviews.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,23 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -67,8 +57,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,26 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
-    <col width="21" customWidth="1" min="10" max="10"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -511,7 +488,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Petrov</t>
+          <t>xesilver</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -523,72 +500,35 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>- Strengths
-  - Implements a straightforward calculator supporting +, -, *, / and handles division by zero by returning an error message.
-  - The core logic is clear and easy to follow. The single calc function is focused and returns results or error messages as designed.
-  - Basic input/output flow is simple and user-friendly for interactive use.
-- Areas for improvement
-  - Input validation and error handling
-    - The code directly casts user input to float without handling invalid numeric input. If a user enters non-numeric text, ValueError will be raised and crash the program.
-    - Consider wrapping input parsing in try/except blocks and provide friendly error messages, then re-prompt.
-  - Consistent return types
-    - calc sometimes returns a numeric result and sometimes a string error message. This can lead to type inconsistencies and require the caller to handle both types.
-    - Prefer one approach: either raise exceptions on error (e.g., ValueError, ZeroDivisionError) or consistently return a result plus an error flag, but avoid mixing types.
-  - Code organization
-    - The script executes I/O at import time. It would be better to guard the interactive block with if __name__ == "__main__": and encapsulate it in a main() function. This makes the module safer to import.
-  - Operator handling
-    - Consider using a dispatch dictionary to map operators to operations. It reduces branching and makes it easier to extend.
-  - Type hints and self-documentation
-    - Adding type hints (def calc(a: float, b: float, op: str) -&gt; float) can improve readability and tooling support.
-  - Documentation and readability
-    - While there is a docstring for calc, adding a module docstring at the top and a short usage example can help users understand how to run the program.
-    - Provide more descriptive parameter names (e.g., a, b could be x, y; though not essential here, it can improve clarity).
-- Suggested improvements (quick wins)
-  - Wrap main execution:
-    - if __name__ == "__main__":
-        main()
-    - def main(): ... includes input parsing with try/except and calls to calc.
-  - Improve calc:
-    - Use a dispatch dictionary, and consider raising exceptions on errors:
-      try:
-          if op == '+': return a + b
-          ...
-          elif op == '/':
-              if b == 0: raise ZeroDivisionError("Division by zero")
-              return a / b
-          else: raise ValueError("Invalid operation")
-      except (ValueError, ZeroDivisionError) as e:
-          return str(e)  # or re-raise, depending on chosen error handling strategy
-  - Add basic unit tests or small assertions to demonstrate expected behavior for key operations.
-Overall, the submission demonstrates correct basic functionality but would benefit from better robustness, clearer error handling, and improved code organization to be production-ready and easier to reuse.</t>
+          <t>Error during review: 'RepositoryService' object has no attribute 'read_student_code'</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-09-14 16:40:50</t>
+          <t>2025-09-19 18:02:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Petrov</t>
+          <t>xesilver</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -600,80 +540,35 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Strengths
-- The core functionality is sound: you can add grades (with validation), compute the average, and display the student’s information.
-- Validation ensures grades stay within 0–100.
-- The average calculation handles the empty-list edge case without crashing.
-Areas for improvement
-- Documentation (0): There are no docstrings for the class or its methods. Adding docstrings will make the code much easier to understand and maintain.
-  - Example: 
-    - class Student: docstring explaining what the class represents.
-    - add_grade/ get_average/ show_grades: brief descriptions of parameters, return values, and side effects.
-- Naming and API design:
-  - The parameter name id shadows Python’s built-in id function. Rename to student_id (and, if desired, annotate types).
-  - Consider adding type hints to improve readability and tooling support, e.g., def __init__(self, name: str, student_id: str) -&gt; None:.
-- Error handling and feedback:
-  - Currently, invalid grades print a message. This is okay for simple scripts, but for robustness consider raising a ValueError or returning a status, so callers can handle errors programmatically.
-  - If you allow floats, ensure you consistently handle them (e.g., ints vs floats). Decide whether grades must be integers.
-- API improvements:
-  - __str__ or __repr__: Implement a string representation so printing the object is informative without needing a separate show_grades method.
-  - Avoid exposing internal state via prints in methods like show_grades. Prefer returning a string or data structure and let the caller decide how to display it.
-- Testing:
-  - Add simple unit tests (e.g., using unittest or pytest) to verify add_grade with valid/invalid inputs, average calculation with no grades, and after several grades.
-- Minor style suggestions:
-  - Add a brief header comment or a module docstring explaining the purpose of the module.
-  - Consider returning a copy of the grades list if you want to protect internal state from external mutation (e.g., in a getter method).
-Suggested enhancements (small code snippets)
-- Rename and type hints:
-  def __init__(self, name: str, student_id: str) -&gt; None:
-      self.name = name
-      self.student_id = student_id
-      self.grades = []
-- Docstring example:
-  class Student:
-      """Represents a student and their grades."""
-      def add_grade(self, grade: float) -&gt; None:
-          """Add a grade (0-100) to the student’s record."""
-          ...
-- Better error handling:
-  def add_grade(self, grade: float) -&gt; None:
-      if not isinstance(grade, (int, float)):
-          raise TypeError("grade must be a number")
-      if not 0 &lt;= grade &lt;= 100:
-          raise ValueError("grade must be between 0 and 100")
-      self.grades.append(grade)
-- __str__ example:
-  def __str__(self) -&gt; str:
-      return f"Student {self.name} (ID: {self.student_id}) - Grades: {self.grades} - Average: {self.get_average()}"
-Overall, you’ve implemented the essential functionality correctly and efficiently. With added documentation, clearer error handling, and a small API polish (renaming id, adding type hints, and providing a nicer string representation), the solution will be much more maintainable and robust.</t>
+          <t>Error during review: 'RepositoryService' object has no attribute 'read_student_code'</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-09-14 16:40:50</t>
+          <t>2025-09-19 18:02:19</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ivanov</t>
+          <t>xesilver</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -681,104 +576,89 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>lecture1_task_1</t>
+          <t>task_1</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>- Strengths
-  - The calculator implements all four basic operations correctly.
-  - Division by zero is properly handled by raising a ValueError, and the CLI catches and reports the error cleanly.
-  - Input handling covers non-numeric input (via float conversion) with a clear error message.
-  - Each function has a docstring detailing purpose, arguments, and return values.
-  - The module is well-structured with a clear main entry point and an under-the-hood separation of concerns (core arithmetic via functions; I/O in main).
--Suggestions for improvement
-  - Add type hints to function signatures to improve readability and enable static checks. Example:
-    def add(a: float, b: float) -&gt; float:
-  - Consider separating the calculator logic from the user interface to facilitate unit testing. For instance, expose a pure function like compute(a, b, op) and have main handle I/O.
-  - Enhance error handling granularity. Right now, a broad catch-all Exception in main can mask programming errors. You could catch specific exceptions (ValueError for conversion/division errors) and let unexpected exceptions propagate or log them.
-  - Add small unit tests (e.g., using pytest) for add, subtract, multiply, divide, and error paths (e.g., divide by zero) to support regression testing.
-  - If you plan to extend features, consider using constants or an Enum for supported operations to avoid string comparisons and improve maintainability.
-  - Optional: provide a minimal README describing how to run the calculator, expected inputs, and examples.
-Overall, a solid implementation suitable for Task 1. With a few cleanups (type hints, modularization, and testing), it would be even more robust and maintainable.</t>
+          <t>- What’s working:
+  - The calculator handles the four basic operations and prints results.
+  - Division by zero is gracefully handled with a message.
+  - Basic input prompts are clear and straightforward.
+- Areas for improvement (technical correctness and robustness):
+  - No input validation beyond division by zero. If a user enters a non-numeric value, float(...) will raise a ValueError and crash the program.
+  - Code mixes calculation logic with I/O (top-level input/output). This makes testing harder and reduces reusability.
+  - There is no main guard (if __name__ == "__main__":). If this file is imported, it will execute immediately, which is undesirable for a library/module.
+  - No unit tests or small testable modules are provided.
+- Suggested improvements:
+  - Add input validation and exception handling for numeric input.
+  - Separate concerns: put calculation logic in pure functions (they already exist) and wrap I/O in a main() function.
+  - Add a main guard to prevent running on import.
+  - Introduce docstrings for functions to explain behavior and types.
+  - Consider using a dispatch map for operations to reduce repetitive conditional logic.
+- Example of improved approach (illustrative, not required to copy exactly):
+  - Include type hints and docstrings.
+  - Use a dict to map operators to functions.
+  - Add a simple main() and a guard.
+  Example (conceptual):
+  def add(x: float, y: float) -&gt; float:
+      """Return the sum of x and y."""
+      return x + y
+  def sub(x: float, y: float) -&gt; float:
+      """Return the difference x - y."""
+      return x - y
+  def mul(x: float, y: float) -&gt; float:
+      """Return the product x * y."""
+      return x * y
+  def div(x: float, y: float) -&gt; float:
+      """Return the division x / y."""
+      return x / y
+  def main():
+      try:
+          a = float(input("Enter first number: "))
+          b = float(input("Enter second number: "))
+      except ValueError:
+          print("Invalid number")
+          return
+      op = input("Enter operation (+, -, *, /): ")
+      ops = {'+': add, '-': sub, '*': mul, '/': div}
+      if op not in ops:
+          print("Invalid operation")
+          return
+      if op == '/' and b == 0:
+          print("Cannot divide by zero")
+          return
+      result = ops[op](a, b)
+      print(result)
+  if __name__ == "__main__":
+      main()
+- Why this helps:
+  - Improves robustness against bad input.
+  - Makes testing easier (you can unit test add, sub, mul, div separately).
+  - Improves readability and maintainability with docstrings and explicit flow control.
+- Additional notes:
+  - Documentation (docstrings) is currently missing. Adding docstrings (and optional type hints) would significantly improve Documentation score.
+  - If this is meant as a standalone script, the current approach is acceptable, but adding a __main__ guard and basic input validation would still be beneficial.</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="G4" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>100</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2025-09-14 16:50:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ivanov</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>lecture1_task_2</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>95</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>- Overall: The implementation is correct and functional. Student and GradeManager behave as expected, with sensible handling of averages and reports.
-- Duplicate IDs: GradeManager.add_student overwrites an existing student with the same ID without warning. Consider guarding against duplicates (e.g., raise an exception or return the existing student) to avoid silent data loss.
-- Type safety: Grades are validated for 0-100, which is good. However, since Python is dynamically typed, passing a non-numeric grade would raise a TypeError during comparison. Consider adding type hints and/or a small type check (isinstance(grade, (int, float))) to provide clearer error messages.
-- Deterministic output: get_grade_report iterates over self.grades.items(), which preserves insertion order in Python 3.7+. If you want deterministic ordering regardless of insertion, consider sorting by subject before printing.
-- Edge cases:
-  - get_class_average returns 0 if there are no students, which is reasonable. If you want to distinguish “no data” from “no grades yet,” you could return None in that case and handle it in the caller.
-  - get_average_grade returns 0 when there are no grades. This is fine, but be aware it can affect class averages if some students have no grades.
-- Readability and style improvements:
-  - Consider adding type hints for all methods and return types to improve readability and enable static analysis.
-  - Could add a __repr__ or __str__ for Student to aid debugging.
-- Documentation: Docstrings are thorough and cover the classes and methods well. That aligns with the provided documentation criteria.
-- Suggested next steps (tests and enhancements):
-  - Write unit tests for:
-    - Adding valid and invalid grades (including boundary values 0 and 100).
-    - get_class_average with no students, with students but no grades, and with mixed grade statuses.
-    - Duplicate student ID behavior.
-    - get_student for existing and non-existing IDs.
-  - Add type hints and maybe input validation in add_student (e.g., ensure ID is a string, name is provided).
-  - Optionally add sorting of subjects in the grade report for deterministic output across runs.</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>95</v>
-      </c>
-      <c r="G5" t="n">
-        <v>90</v>
-      </c>
-      <c r="H5" t="n">
-        <v>100</v>
-      </c>
-      <c r="I5" t="n">
-        <v>100</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2025-09-14 16:50:56</t>
+          <t>2025-09-19 18:08:39</t>
         </is>
       </c>
     </row>

</xml_diff>